<commit_message>
Gata cu SCR ul finally
</commit_message>
<xml_diff>
--- a/Test/BagaAici/Catalog/SCR_new_201910.xlsx
+++ b/Test/BagaAici/Catalog/SCR_new_201910.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei Bancila\Desktop\sadf\FurnizoriClean\Fisiere\SCR\Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei Bancila\Desktop\SupplierListManagerProject\Test\BagaAici\Catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A59119F-A322-4E38-9677-1FCAECD9B537}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388579D6-EBE3-435D-94D6-DAC198BD8C61}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="108">
   <si>
     <t>Art.No.</t>
   </si>
@@ -344,6 +344,9 @@
   </si>
   <si>
     <t>1770131770131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">si </t>
   </si>
 </sst>
 </file>
@@ -749,7 +752,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.21875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1174,6 +1177,9 @@
       <c r="K11" s="12" t="s">
         <v>57</v>
       </c>
+      <c r="M11" s="13" t="s">
+        <v>107</v>
+      </c>
       <c r="N11" s="13" t="s">
         <v>88</v>
       </c>

</xml_diff>